<commit_message>
First commit to camnieve. Pulled from Alvin Merto's git repository.
</commit_message>
<xml_diff>
--- a/public/Inspection and Acceptance Report.xlsx
+++ b/public/Inspection and Acceptance Report.xlsx
@@ -7,7 +7,7 @@
     <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="IAR LIST" sheetId="1" r:id="rId4"/>
+    <sheet name="IAR" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="1" fullCalcOnLoad="0" forceFullCalc="0"/>
@@ -15,9 +15,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="21">
-  <si>
-    <t>LIST OF INSPECTION AND ACCEPTANCE REPORT</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="39">
+  <si>
+    <t>Appendix 62</t>
+  </si>
+  <si>
+    <t>INSPECTION AND ACCEPTANCE REPORT</t>
   </si>
   <si>
     <t>Entity Name : MINDANAO DEVELOPMENT AUTHORITY</t>
@@ -26,58 +29,110 @@
     <t>Fund Cluster : 101</t>
   </si>
   <si>
-    <t>PO No./Date</t>
-  </si>
-  <si>
-    <t>IAR No.</t>
-  </si>
-  <si>
-    <t>Supplier</t>
-  </si>
-  <si>
-    <t>Requisitioning Office/Dept.</t>
-  </si>
-  <si>
-    <t>Respo Center Code</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 63453535345</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 2020-0005</t>
-  </si>
-  <si>
-    <t>Computer World</t>
-  </si>
-  <si>
-    <t>AD Continuing</t>
+    <t>Supplier :</t>
+  </si>
+  <si>
+    <t>V.S. Tay Supplies</t>
+  </si>
+  <si>
+    <t>IAR No. :</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2022-0002</t>
+  </si>
+  <si>
+    <t>PO No./Date :</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 345235345</t>
+  </si>
+  <si>
+    <t>Date :</t>
+  </si>
+  <si>
+    <t>1/10/2022</t>
+  </si>
+  <si>
+    <t>Requisitioning Office/Dept. :</t>
+  </si>
+  <si>
+    <t>KMD Regular</t>
+  </si>
+  <si>
+    <t>Invoice No. :</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 34535345</t>
+  </si>
+  <si>
+    <t>Respo Center Code :</t>
+  </si>
+  <si>
+    <t>KMD ISSP PuRD 200000100002</t>
+  </si>
+  <si>
+    <t>Stock/
+Property No.</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Unit/Cost</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>as scdsfd safsdfdf dsaf</t>
+  </si>
+  <si>
+    <t>(pcs) 1,000.00</t>
+  </si>
+  <si>
+    <t>asdfsafasdfs</t>
+  </si>
+  <si>
+    <t>(box) 100.00</t>
+  </si>
+  <si>
+    <t>INSPECTION</t>
+  </si>
+  <si>
+    <t>ACCEPTANCE</t>
+  </si>
+  <si>
+    <t>Date Inspected : 1/10/2022</t>
+  </si>
+  <si>
+    <t>Date Received : 1/10/2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Inspected, verified and found in order as to quantity and specifications</t>
+  </si>
+  <si>
+    <t>R</t>
   </si>
   <si>
     <t>Completed</t>
   </si>
   <si>
-    <t xml:space="preserve"> 2354345435435</t>
-  </si>
-  <si>
-    <t>ertwetetewt</t>
-  </si>
-  <si>
-    <t>IPD Continuing</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 2019-12-667</t>
-  </si>
-  <si>
-    <t>ENENS ORNAMENTAL GARDEN</t>
-  </si>
-  <si>
-    <t>AD Regular</t>
-  </si>
-  <si>
-    <t>************************** NOTHING FOLLOWS **************************</t>
+    <t>*</t>
+  </si>
+  <si>
+    <t>Partial (pls. specify quantity)</t>
+  </si>
+  <si>
+    <t>WERCWEREWR</t>
+  </si>
+  <si>
+    <t>WWERECEREWR</t>
+  </si>
+  <si>
+    <t>wecrwer</t>
+  </si>
+  <si>
+    <t>wercwerwer</t>
   </si>
 </sst>
 </file>
@@ -85,7 +140,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="8">
     <font>
       <b val="0"/>
       <i val="0"/>
@@ -100,9 +155,63 @@
       <i val="1"/>
       <strike val="0"/>
       <u val="none"/>
+      <sz val="14"/>
+      <color rgb="FF3b5998"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <i val="1"/>
+      <strike val="0"/>
+      <u val="none"/>
       <sz val="11"/>
       <color rgb="FFffffff"/>
       <name val="Times New Roman"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <i val="1"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Wingdings 2"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="3">
@@ -110,56 +219,376 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="3b5998"/>
+        <fgColor rgb="FF3b5998"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="24">
     <border/>
     <border>
-      <left style="thin">
-        <color rgb="000000"/>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color rgb="000000"/>
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
       </right>
       <top style="thin">
-        <color rgb="000000"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
-        <color rgb="000000"/>
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
+    <border>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
+    <border>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+    </border>
+    <border>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
       </bottom>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="47">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+      <alignment vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
+      <alignment vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="2" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="2" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="3" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="4" numFmtId="0" fillId="2" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="5" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="5" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="5" numFmtId="0" fillId="0" borderId="5" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="0" borderId="5" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="0" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="6" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="7" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="8" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="4" numFmtId="0" fillId="2" borderId="9" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="10" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="10" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="5" numFmtId="0" fillId="0" borderId="10" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="0" borderId="10" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="11" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="11" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="0" borderId="11" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="12" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="6" numFmtId="0" fillId="0" borderId="13" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="13" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="0" borderId="13" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="14" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="15" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="16" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="17" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="7" numFmtId="0" fillId="0" borderId="10" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="18" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="19" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="20" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="4" numFmtId="0" fillId="2" borderId="21" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="7" numFmtId="0" fillId="0" borderId="22" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="22" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="5" numFmtId="0" fillId="0" borderId="22" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="0" borderId="22" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="0" borderId="19" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="23" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -456,146 +885,319 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A7" sqref="A7:F10"/>
+      <selection activeCell="A5" sqref="A5:F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="17.22" customWidth="true" style="0"/>
-    <col min="2" max="2" width="13.44" customWidth="true" style="0"/>
-    <col min="3" max="3" width="28" customWidth="true" style="0"/>
-    <col min="4" max="4" width="18" customWidth="true" style="0"/>
-    <col min="5" max="5" width="18" customWidth="true" style="0"/>
+    <col min="2" max="2" width="44.22" customWidth="true" style="0"/>
+    <col min="3" max="3" width="3.33" customWidth="true" style="0"/>
+    <col min="4" max="4" width="12.67" customWidth="true" style="0"/>
+    <col min="5" max="5" width="8.11" customWidth="true" style="0"/>
     <col min="6" max="6" width="13.33" customWidth="true" style="0"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1"/>
+    </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="1" t="s">
+      <c r="A2"/>
+      <c r="D2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3"/>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" t="s">
+      <c r="A4"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D4" t="s">
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+    </row>
+    <row r="6" spans="1:6" customHeight="1" ht="31.22">
+      <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" customHeight="1" ht="35">
-      <c r="A6" s="2" t="s">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+    </row>
+    <row r="8" spans="1:6" customHeight="1" ht="22">
+      <c r="A8" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="B8" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="C8" s="17"/>
+      <c r="D8" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E8" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F8" s="37"/>
+    </row>
+    <row r="9" spans="1:6" customHeight="1" ht="22">
+      <c r="A9" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" customHeight="1" ht="25">
-      <c r="A7" s="3" t="s">
+      <c r="B9" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="C9" s="4"/>
+      <c r="D9" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="E9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="F9" s="38"/>
+    </row>
+    <row r="10" spans="1:6" customHeight="1" ht="22">
+      <c r="A10" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="4" t="s">
+      <c r="B10" s="4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" customHeight="1" ht="25">
-      <c r="A8" s="3" t="s">
+      <c r="C10" s="4"/>
+      <c r="D10" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="E10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="38"/>
+    </row>
+    <row r="11" spans="1:6" customHeight="1" ht="22">
+      <c r="A11" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="4"/>
+      <c r="D11" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="E11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="38"/>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="8"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="39"/>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" s="40"/>
+    </row>
+    <row r="14" spans="1:6" customHeight="1" ht="25">
+      <c r="A14" s="10"/>
+      <c r="B14" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="20"/>
+      <c r="D14" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" s="36">
         <v>15</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" customHeight="1" ht="25">
-      <c r="A9" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" customHeight="1" ht="31.2">
-      <c r="A10" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-    </row>
-    <row r="11" spans="1:6" customHeight="1" ht="22"/>
+      <c r="F14" s="41"/>
+    </row>
+    <row r="15" spans="1:6" customHeight="1" ht="25">
+      <c r="A15" s="10"/>
+      <c r="B15" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="20"/>
+      <c r="D15" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" s="36">
+        <v>50</v>
+      </c>
+      <c r="F15" s="41"/>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="11"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="42"/>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="22"/>
+      <c r="C17" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="43"/>
+    </row>
+    <row r="18" spans="1:6" customHeight="1" ht="31.2">
+      <c r="A18" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="23"/>
+      <c r="C18" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="44"/>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="24"/>
+      <c r="C19" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E19" s="4"/>
+      <c r="F19" s="38"/>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="7"/>
+      <c r="B20" s="24"/>
+      <c r="C20" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E20" s="4"/>
+      <c r="F20" s="38"/>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="7"/>
+      <c r="B21" s="24"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="38"/>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="6"/>
+      <c r="B22" s="25"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="38"/>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" s="26"/>
+      <c r="C23" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" s="34"/>
+      <c r="E23" s="34"/>
+      <c r="F23" s="45"/>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="27"/>
+      <c r="C24" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24" s="35"/>
+      <c r="E24" s="35"/>
+      <c r="F24" s="46"/>
+    </row>
   </sheetData>
-  <sheetProtection password="E94D" sheet="true" objects="false" scenarios="false" formatCells="true" formatColumns="false" formatRows="false" insertColumns="false" insertRows="true" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="true" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
+  <sheetProtection password="8D7A" sheet="true" objects="false" scenarios="false" formatCells="true" formatColumns="false" formatRows="false" insertColumns="false" insertRows="true" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="true" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <mergeCells>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="A5:F5"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="A16:F16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="C17:F17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="A19:B21"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="C23:F23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="C24:F24"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1"/>
+  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
   <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
     <oddHeader/>
     <oddFooter/>
@@ -604,5 +1206,6 @@
     <firstHeader/>
     <firstFooter/>
   </headerFooter>
+  <tableParts count="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Change IAR submenu items to treeview
</commit_message>
<xml_diff>
--- a/public/Inspection and Acceptance Report.xlsx
+++ b/public/Inspection and Acceptance Report.xlsx
@@ -32,25 +32,25 @@
     <t>Supplier :</t>
   </si>
   <si>
-    <t>V.S. Tay Supplies</t>
+    <t>Cameron Nieve</t>
   </si>
   <si>
     <t>IAR No. :</t>
   </si>
   <si>
-    <t xml:space="preserve"> 2022-0002</t>
+    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>PO No./Date :</t>
   </si>
   <si>
-    <t xml:space="preserve"> 345235345</t>
+    <t xml:space="preserve"> 2022-099283</t>
   </si>
   <si>
     <t>Date :</t>
   </si>
   <si>
-    <t>1/10/2022</t>
+    <t>1/10/2023</t>
   </si>
   <si>
     <t>Requisitioning Office/Dept. :</t>
@@ -62,13 +62,16 @@
     <t>Invoice No. :</t>
   </si>
   <si>
-    <t xml:space="preserve"> 34535345</t>
+    <t xml:space="preserve"> 12345678</t>
   </si>
   <si>
     <t>Respo Center Code :</t>
   </si>
   <si>
-    <t>KMD ISSP PuRD 200000100002</t>
+    <t>AMO 310200100000</t>
+  </si>
+  <si>
+    <t>12/21/2022</t>
   </si>
   <si>
     <t>Stock/
@@ -90,37 +93,34 @@
     <t>(pcs) 1,000.00</t>
   </si>
   <si>
-    <t>asdfsafasdfs</t>
-  </si>
-  <si>
-    <t>(box) 100.00</t>
-  </si>
-  <si>
     <t>INSPECTION</t>
   </si>
   <si>
     <t>ACCEPTANCE</t>
   </si>
   <si>
-    <t>Date Inspected : 1/10/2022</t>
-  </si>
-  <si>
-    <t>Date Received : 1/10/2022</t>
+    <t>Date Inspected : 1/10/2023</t>
+  </si>
+  <si>
+    <t>Date Received : 1/10/2023</t>
   </si>
   <si>
     <t xml:space="preserve">     Inspected, verified and found in order as to quantity and specifications</t>
   </si>
   <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
     <t>R</t>
   </si>
   <si>
-    <t>Completed</t>
-  </si>
-  <si>
-    <t>*</t>
-  </si>
-  <si>
     <t>Partial (pls. specify quantity)</t>
+  </si>
+  <si>
+    <t>Partial quantity: 0</t>
   </si>
   <si>
     <t>WERCWEREWR</t>
@@ -228,7 +228,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="29">
     <border/>
     <border>
       <left style="medium">
@@ -286,6 +286,14 @@
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
@@ -332,11 +340,19 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
     </border>
     <border>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
@@ -348,11 +364,19 @@
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
@@ -380,6 +404,11 @@
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+    </border>
+    <border>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
@@ -432,6 +461,14 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+    </border>
+    <border>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
     </border>
     <border>
       <right style="medium">
@@ -448,7 +485,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="52">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
@@ -491,35 +528,26 @@
     <xf xfId="0" fontId="3" numFmtId="0" fillId="0" borderId="5" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="6" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
     <xf xfId="0" fontId="3" numFmtId="0" fillId="0" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="6" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="7" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="7" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="8" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="4" numFmtId="0" fillId="2" borderId="9" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="9" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="4" numFmtId="0" fillId="2" borderId="10" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="10" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="10" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="5" numFmtId="0" fillId="0" borderId="10" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="0" fillId="0" borderId="10" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="11" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
@@ -527,14 +555,17 @@
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="11" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
+    <xf xfId="0" fontId="5" numFmtId="0" fillId="0" borderId="11" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
     <xf xfId="0" fontId="3" numFmtId="0" fillId="0" borderId="11" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+      <alignment vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="12" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="6" numFmtId="0" fillId="0" borderId="13" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+      <alignment vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="13" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="13" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
@@ -545,49 +576,70 @@
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="14" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="15" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="6" numFmtId="0" fillId="0" borderId="15" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="6" numFmtId="0" fillId="0" borderId="16" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="16" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="0" borderId="16" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="17" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="18" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="19" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="20" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="3" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="17" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="21" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="7" numFmtId="0" fillId="0" borderId="10" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="7" numFmtId="0" fillId="0" borderId="11" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="18" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="19" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="20" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="4" numFmtId="0" fillId="2" borderId="21" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="22" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="23" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="24" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="4" numFmtId="0" fillId="2" borderId="25" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="7" numFmtId="0" fillId="0" borderId="22" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="7" numFmtId="0" fillId="0" borderId="26" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="22" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="5" numFmtId="0" fillId="0" borderId="22" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="26" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="5" numFmtId="0" fillId="0" borderId="26" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="3" numFmtId="0" fillId="0" borderId="22" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="0" fillId="0" borderId="19" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="0" borderId="26" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="27" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="0" borderId="23" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="23" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="28" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
   </cellXfs>
@@ -889,10 +941,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A5" sqref="A5:F24"/>
+      <selection activeCell="A5" sqref="A5:F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -924,11 +976,11 @@
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
     </row>
     <row r="6" spans="1:6" customHeight="1" ht="31.22">
       <c r="A6" s="3" t="s">
@@ -954,17 +1006,17 @@
       <c r="A8" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="17"/>
-      <c r="D8" s="32" t="s">
+      <c r="C8" s="18"/>
+      <c r="D8" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="17" t="s">
+      <c r="E8" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="37"/>
+      <c r="F8" s="41"/>
     </row>
     <row r="9" spans="1:6" customHeight="1" ht="22">
       <c r="A9" s="6" t="s">
@@ -974,13 +1026,13 @@
         <v>9</v>
       </c>
       <c r="C9" s="4"/>
-      <c r="D9" s="29" t="s">
+      <c r="D9" s="32" t="s">
         <v>10</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="38"/>
+      <c r="F9" s="42"/>
     </row>
     <row r="10" spans="1:6" customHeight="1" ht="22">
       <c r="A10" s="7" t="s">
@@ -990,13 +1042,13 @@
         <v>13</v>
       </c>
       <c r="C10" s="4"/>
-      <c r="D10" s="29" t="s">
+      <c r="D10" s="32" t="s">
         <v>14</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="38"/>
+      <c r="F10" s="42"/>
     </row>
     <row r="11" spans="1:6" customHeight="1" ht="22">
       <c r="A11" s="6" t="s">
@@ -1006,166 +1058,176 @@
         <v>17</v>
       </c>
       <c r="C11" s="4"/>
-      <c r="D11" s="29" t="s">
+      <c r="D11" s="32" t="s">
         <v>10</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" s="38"/>
+        <v>18</v>
+      </c>
+      <c r="F11" s="42"/>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="8"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="33"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="39"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="43"/>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19" t="s">
+      <c r="B13" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="19" t="s">
+      <c r="C13" s="20"/>
+      <c r="D13" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="F13" s="40"/>
+      <c r="E13" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" s="44"/>
     </row>
     <row r="14" spans="1:6" customHeight="1" ht="25">
       <c r="A14" s="10"/>
-      <c r="B14" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="20"/>
-      <c r="D14" s="21" t="s">
+      <c r="B14" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="E14" s="36">
-        <v>15</v>
-      </c>
-      <c r="F14" s="41"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" s="40">
+        <v>5</v>
+      </c>
+      <c r="F14" s="45"/>
     </row>
     <row r="15" spans="1:6" customHeight="1" ht="25">
       <c r="A15" s="10"/>
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="21"/>
+      <c r="D15" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="20"/>
-      <c r="D15" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="E15" s="36">
-        <v>50</v>
-      </c>
-      <c r="F15" s="41"/>
+      <c r="E15" s="40">
+        <v>5</v>
+      </c>
+      <c r="F15" s="45"/>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="11"/>
-      <c r="B16" s="21"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="42"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="46"/>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="23"/>
+      <c r="C17" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="22"/>
-      <c r="C17" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="D17" s="22"/>
-      <c r="E17" s="22"/>
-      <c r="F17" s="43"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="47"/>
     </row>
     <row r="18" spans="1:6" customHeight="1" ht="31.2">
       <c r="A18" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="24"/>
+      <c r="C18" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="B18" s="23"/>
-      <c r="C18" s="23" t="s">
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="48"/>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="23"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="44"/>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="7" t="s">
+      <c r="B19" s="25"/>
+      <c r="C19" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="B19" s="24"/>
-      <c r="C19" s="28" t="s">
+      <c r="D19" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="D19" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E19" s="4"/>
-      <c r="F19" s="38"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="49"/>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="7"/>
-      <c r="B20" s="24"/>
-      <c r="C20" s="28" t="s">
+      <c r="B20" s="26"/>
+      <c r="C20" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D20" s="4" t="s">
-        <v>34</v>
-      </c>
       <c r="E20" s="4"/>
-      <c r="F20" s="38"/>
+      <c r="F20" s="42"/>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="7"/>
-      <c r="B21" s="24"/>
-      <c r="C21" s="29"/>
-      <c r="D21" s="4"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="32"/>
+      <c r="D21" s="4" t="s">
+        <v>34</v>
+      </c>
       <c r="E21" s="4"/>
-      <c r="F21" s="38"/>
+      <c r="F21" s="42"/>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="6"/>
-      <c r="B22" s="25"/>
-      <c r="C22" s="29"/>
+      <c r="B22" s="27"/>
+      <c r="C22" s="32"/>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
-      <c r="F22" s="38"/>
+      <c r="F22" s="42"/>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="B23" s="26"/>
-      <c r="C23" s="30" t="s">
-        <v>36</v>
-      </c>
-      <c r="D23" s="34"/>
-      <c r="E23" s="34"/>
-      <c r="F23" s="45"/>
+      <c r="A23" s="6"/>
+      <c r="B23" s="27"/>
+      <c r="C23" s="32"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="42"/>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" s="28"/>
+      <c r="C24" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="D24" s="38"/>
+      <c r="E24" s="38"/>
+      <c r="F24" s="50"/>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="B24" s="27"/>
-      <c r="C24" s="31" t="s">
+      <c r="B25" s="29"/>
+      <c r="C25" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="D24" s="35"/>
-      <c r="E24" s="35"/>
-      <c r="F24" s="46"/>
+      <c r="D25" s="39"/>
+      <c r="E25" s="39"/>
+      <c r="F25" s="51"/>
     </row>
   </sheetData>
-  <sheetProtection password="8D7A" sheet="true" objects="false" scenarios="false" formatCells="true" formatColumns="false" formatRows="false" insertColumns="false" insertRows="true" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="true" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
+  <sheetProtection password="F065" sheet="true" objects="false" scenarios="false" formatCells="true" formatColumns="false" formatRows="false" insertColumns="false" insertRows="true" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="true" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <mergeCells>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A2:C2"/>
@@ -1190,10 +1252,10 @@
     <mergeCell ref="C18:F18"/>
     <mergeCell ref="A19:B21"/>
     <mergeCell ref="D20:F20"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="C23:F23"/>
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="C24:F24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="C25:F25"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>